<commit_message>
complete final php labs
</commit_message>
<xml_diff>
--- a/backend/app/lab4/test.xlsx
+++ b/backend/app/lab4/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Для учебы\4 семестр\WEB-INTARO\project-PHP-WEB\backend\app\lab4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F935B13F-DEA7-44B1-A4DA-B6B7B75BFAA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64673F01-662C-423D-9C94-74D1798E3171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="180" yWindow="360" windowWidth="20568" windowHeight="11340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1021,8 +1021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>